<commit_message>
contains list of assumptions
</commit_message>
<xml_diff>
--- a/irrigation_assumptions_SM.xlsx
+++ b/irrigation_assumptions_SM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bham-my.sharepoint.com/personal/sxl1405_student_bham_ac_uk/Documents/dawn/1assumptionhunting/supervisors_review/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{575441F0-2342-6942-AE23-487E9AD19909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{201D61C3-AA06-3840-BDE4-7DEBE72CA913}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{575441F0-2342-6942-AE23-487E9AD19909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D86A8F0F-477B-8344-A22B-2EF5F969FF03}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="17520" activeTab="1" xr2:uid="{2B59B78E-27CF-CD4A-8C23-D643904316C3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{2B59B78E-27CF-CD4A-8C23-D643904316C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="39" r:id="rId1"/>
@@ -1013,6 +1013,9 @@
     <t>Irrigation efficiency for groundwater irrigation is set to 0.7 globally</t>
   </si>
   <si>
+    <t>Supplementary Material for: Global irrigation modelling relies more on pragmatic than empirical assumptions</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Authors: </t>
     </r>
@@ -1042,11 +1045,8 @@
         <rFont val="Aptos Narrow"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, Carmen Aguiló, Joshua Larsen, Michela Massimi, Nanxin Wei, Arnald Puy</t>
+      <t>, Carmen Aguiló-Rivera, Joshua Larsen, Michela Massimi, Nanxin Wei, and Arnald Puy</t>
     </r>
-  </si>
-  <si>
-    <t>Supplementary Material for: Global irrigation modelling relies more on pragmatic than empirical assumptions</t>
   </si>
 </sst>
 </file>
@@ -1386,6 +1386,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1729,15 +1733,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48B5257C-4D59-5740-AC26-75B13285ECA3}">
   <dimension ref="A2:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="B2" s="12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
@@ -1753,7 +1757,7 @@
     <row r="4" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="13" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
@@ -1883,7 +1887,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB67CFA7-4902-9745-888A-DE1C4E0A62CA}">
   <dimension ref="A1:P115"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>

</xml_diff>